<commit_message>
add history to ex 2
</commit_message>
<xml_diff>
--- a/Raspisanie-FIT-ochnaya-f.o-23_24-vesenniy-sem.-APREL.xlsx
+++ b/Raspisanie-FIT-ochnaya-f.o-23_24-vesenniy-sem.-APREL.xlsx
@@ -558,70 +558,6 @@
       </diagonal>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="00000000"/>
       </left>
@@ -682,6 +618,70 @@
       <diagonal>
         <color rgb="00000000"/>
       </diagonal>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left>
@@ -909,7 +909,7 @@
       <alignment horizontal="general" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -924,13 +924,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -941,7 +941,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="11" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -960,7 +960,7 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
@@ -975,7 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -986,7 +986,7 @@
       <alignment horizontal="center" vertical="bottom"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
@@ -1002,7 +1002,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
@@ -1229,10 +1229,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -5916,39 +5916,39 @@
   <mergeCells count="219">
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="B196:B207"/>
+    <mergeCell ref="C210:C211"/>
+    <mergeCell ref="C184:C185"/>
     <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C184:C185"/>
-    <mergeCell ref="C210:C211"/>
     <mergeCell ref="C250:C251"/>
     <mergeCell ref="C146:C147"/>
     <mergeCell ref="A156:A167"/>
+    <mergeCell ref="C234:C235"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="C274:C275"/>
     <mergeCell ref="C134:C135"/>
+    <mergeCell ref="C252:C253"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C252:C253"/>
-    <mergeCell ref="C274:C275"/>
     <mergeCell ref="B296:B307"/>
     <mergeCell ref="A220:A231"/>
     <mergeCell ref="A247:C247"/>
     <mergeCell ref="C114:C115"/>
     <mergeCell ref="C242:C243"/>
+    <mergeCell ref="C276:C277"/>
     <mergeCell ref="C236:C237"/>
-    <mergeCell ref="C276:C277"/>
     <mergeCell ref="C214:C215"/>
     <mergeCell ref="C132:C133"/>
     <mergeCell ref="B56:B67"/>
     <mergeCell ref="B184:B195"/>
     <mergeCell ref="C226:C227"/>
+    <mergeCell ref="B32:B43"/>
     <mergeCell ref="C164:C165"/>
-    <mergeCell ref="B32:B43"/>
     <mergeCell ref="C300:C301"/>
     <mergeCell ref="A171:C171"/>
     <mergeCell ref="C278:C279"/>
     <mergeCell ref="B120:B131"/>
     <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C228:C229"/>
     <mergeCell ref="B96:B107"/>
-    <mergeCell ref="C228:C229"/>
     <mergeCell ref="C222:C223"/>
     <mergeCell ref="C66:C67"/>
     <mergeCell ref="C262:C263"/>
@@ -5980,27 +5980,27 @@
     <mergeCell ref="C218:C219"/>
     <mergeCell ref="A168:A169"/>
     <mergeCell ref="C230:C231"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="A308:A319"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="C168:C169"/>
+    <mergeCell ref="A95:C95"/>
+    <mergeCell ref="A68:A79"/>
     <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="A68:A79"/>
-    <mergeCell ref="A95:C95"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="A308:A319"/>
     <mergeCell ref="C100:C101"/>
     <mergeCell ref="C152:C153"/>
+    <mergeCell ref="A132:A143"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A132:A143"/>
+    <mergeCell ref="C272:C273"/>
     <mergeCell ref="C148:C149"/>
-    <mergeCell ref="C272:C273"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A260:A271"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C282:C283"/>
     <mergeCell ref="C138:C139"/>
     <mergeCell ref="C316:C317"/>
+    <mergeCell ref="C120:C121"/>
     <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C120:C121"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A170:C170"/>
     <mergeCell ref="A284:A295"/>
@@ -6008,8 +6008,8 @@
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C244:C245"/>
     <mergeCell ref="B208:B219"/>
+    <mergeCell ref="C140:C141"/>
     <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C140:C141"/>
     <mergeCell ref="B168:B169"/>
     <mergeCell ref="D168:E168"/>
     <mergeCell ref="C32:C33"/>
@@ -6023,63 +6023,63 @@
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="A92:A93"/>
     <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C126:C127"/>
     <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C126:C127"/>
     <mergeCell ref="C310:C311"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A20:A31"/>
+    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C116:C117"/>
     <mergeCell ref="C294:C295"/>
     <mergeCell ref="C216:C217"/>
     <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="A184:A195"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A184:A195"/>
-    <mergeCell ref="C284:C285"/>
     <mergeCell ref="C318:C319"/>
     <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B284:B295"/>
+    <mergeCell ref="C280:C281"/>
     <mergeCell ref="B20:B31"/>
-    <mergeCell ref="C280:C281"/>
-    <mergeCell ref="B284:B295"/>
     <mergeCell ref="B244:B245"/>
     <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C44:C45"/>
     <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C286:C287"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C286:C287"/>
     <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A96:A107"/>
     <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A96:A107"/>
-    <mergeCell ref="C202:C203"/>
     <mergeCell ref="A232:A243"/>
     <mergeCell ref="C270:C271"/>
     <mergeCell ref="C192:C193"/>
     <mergeCell ref="B156:B167"/>
     <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B248:B259"/>
     <mergeCell ref="C238:C239"/>
     <mergeCell ref="C176:C177"/>
-    <mergeCell ref="B248:B259"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="A172:A183"/>
+    <mergeCell ref="D244:E244"/>
     <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D244:E244"/>
     <mergeCell ref="C312:C313"/>
     <mergeCell ref="C194:C195"/>
     <mergeCell ref="B232:B243"/>
     <mergeCell ref="B272:B283"/>
+    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="C296:C297"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="C78:C79"/>
     <mergeCell ref="A56:A67"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="C240:C241"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C296:C297"/>
     <mergeCell ref="C258:C259"/>
     <mergeCell ref="C314:C315"/>
     <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="C106:C107"/>
     <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C224:C225"/>
     <mergeCell ref="C298:C299"/>
     <mergeCell ref="D92:E92"/>
     <mergeCell ref="C38:C39"/>
@@ -6088,8 +6088,8 @@
     <mergeCell ref="C204:C205"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="C154:C155"/>
+    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C172:C173"/>
-    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C206:C207"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="C156:C157"/>
@@ -6097,27 +6097,27 @@
     <mergeCell ref="C196:C197"/>
     <mergeCell ref="B260:B271"/>
     <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C302:C303"/>
     <mergeCell ref="C180:C181"/>
-    <mergeCell ref="C302:C303"/>
     <mergeCell ref="C118:C119"/>
     <mergeCell ref="B144:B155"/>
     <mergeCell ref="C198:C199"/>
     <mergeCell ref="C90:C91"/>
     <mergeCell ref="C130:C131"/>
     <mergeCell ref="C182:C183"/>
+    <mergeCell ref="C110:C111"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C110:C111"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="C150:C151"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="C232:C233"/>
     <mergeCell ref="B132:B143"/>
     <mergeCell ref="C72:C73"/>
+    <mergeCell ref="B220:B231"/>
     <mergeCell ref="C96:C97"/>
-    <mergeCell ref="B220:B231"/>
     <mergeCell ref="C208:C209"/>
     <mergeCell ref="A120:A131"/>
     <mergeCell ref="C158:C159"/>
@@ -6125,11 +6125,11 @@
     <mergeCell ref="A94:C94"/>
     <mergeCell ref="B44:B55"/>
     <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C186:C187"/>
     <mergeCell ref="C108:C109"/>
-    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C200:C201"/>
     <mergeCell ref="C266:C267"/>
     <mergeCell ref="C260:C261"/>
     <mergeCell ref="C92:C93"/>
@@ -9736,32 +9736,32 @@
   <mergeCells count="215">
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="A234:A245"/>
+    <mergeCell ref="C210:C211"/>
+    <mergeCell ref="C184:C185"/>
     <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C184:C185"/>
-    <mergeCell ref="C210:C211"/>
     <mergeCell ref="C250:C251"/>
     <mergeCell ref="C146:C147"/>
     <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C234:C235"/>
     <mergeCell ref="A21:C21"/>
-    <mergeCell ref="C234:C235"/>
-    <mergeCell ref="C134:C135"/>
+    <mergeCell ref="C274:C275"/>
     <mergeCell ref="B198:B209"/>
     <mergeCell ref="C252:C253"/>
-    <mergeCell ref="C274:C275"/>
+    <mergeCell ref="C134:C135"/>
     <mergeCell ref="B134:B145"/>
     <mergeCell ref="C114:C115"/>
     <mergeCell ref="C242:C243"/>
+    <mergeCell ref="C276:C277"/>
     <mergeCell ref="C236:C237"/>
-    <mergeCell ref="C276:C277"/>
     <mergeCell ref="C214:C215"/>
     <mergeCell ref="B122:B133"/>
     <mergeCell ref="C132:C133"/>
     <mergeCell ref="C226:C227"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="C164:C165"/>
-    <mergeCell ref="D16:D17"/>
     <mergeCell ref="C300:C301"/>
+    <mergeCell ref="C278:C279"/>
     <mergeCell ref="B246:B247"/>
-    <mergeCell ref="C278:C279"/>
     <mergeCell ref="A110:A121"/>
     <mergeCell ref="C188:C189"/>
     <mergeCell ref="C228:C229"/>
@@ -9770,37 +9770,37 @@
     <mergeCell ref="C262:C263"/>
     <mergeCell ref="A173:C173"/>
     <mergeCell ref="A174:A185"/>
+    <mergeCell ref="C190:C191"/>
     <mergeCell ref="B58:B69"/>
-    <mergeCell ref="C190:C191"/>
     <mergeCell ref="B98:B109"/>
     <mergeCell ref="C86:C87"/>
     <mergeCell ref="C264:C265"/>
+    <mergeCell ref="B234:B245"/>
     <mergeCell ref="A158:A169"/>
-    <mergeCell ref="B234:B245"/>
     <mergeCell ref="C174:C175"/>
     <mergeCell ref="A298:A309"/>
+    <mergeCell ref="C254:C255"/>
     <mergeCell ref="B82:B93"/>
-    <mergeCell ref="C254:C255"/>
     <mergeCell ref="A46:A57"/>
     <mergeCell ref="C304:C305"/>
     <mergeCell ref="B146:B157"/>
     <mergeCell ref="C98:C99"/>
     <mergeCell ref="C256:C257"/>
     <mergeCell ref="A210:A221"/>
+    <mergeCell ref="B34:B45"/>
     <mergeCell ref="C166:C167"/>
-    <mergeCell ref="B34:B45"/>
     <mergeCell ref="A246:A247"/>
+    <mergeCell ref="C306:C307"/>
     <mergeCell ref="B174:B185"/>
-    <mergeCell ref="C306:C307"/>
     <mergeCell ref="C162:C163"/>
     <mergeCell ref="C218:C219"/>
     <mergeCell ref="B170:B171"/>
     <mergeCell ref="A274:A285"/>
     <mergeCell ref="C230:C231"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="C290:C291"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="C168:C169"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="C290:C291"/>
     <mergeCell ref="A248:C248"/>
     <mergeCell ref="B110:B121"/>
     <mergeCell ref="C100:C101"/>
@@ -9808,29 +9808,29 @@
     <mergeCell ref="C152:C153"/>
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="A310:A321"/>
+    <mergeCell ref="C272:C273"/>
+    <mergeCell ref="C148:C149"/>
     <mergeCell ref="A97:C97"/>
-    <mergeCell ref="C148:C149"/>
-    <mergeCell ref="C272:C273"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="B22:B33"/>
     <mergeCell ref="C282:C283"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="C316:C317"/>
+    <mergeCell ref="C120:C121"/>
     <mergeCell ref="A96:C96"/>
-    <mergeCell ref="C138:C139"/>
     <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="C316:C317"/>
     <mergeCell ref="A222:A233"/>
     <mergeCell ref="A249:C249"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C244:C245"/>
+    <mergeCell ref="C140:C141"/>
     <mergeCell ref="C82:C83"/>
-    <mergeCell ref="C140:C141"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A286:A297"/>
     <mergeCell ref="C268:C269"/>
     <mergeCell ref="B70:B81"/>
-    <mergeCell ref="A286:A297"/>
     <mergeCell ref="C308:C309"/>
     <mergeCell ref="C102:C103"/>
     <mergeCell ref="B210:B221"/>
@@ -9838,67 +9838,68 @@
     <mergeCell ref="C292:C293"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="C310:C311"/>
     <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="C310:C311"/>
     <mergeCell ref="A198:A209"/>
+    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B310:B321"/>
+    <mergeCell ref="B186:B197"/>
+    <mergeCell ref="A172:C172"/>
+    <mergeCell ref="C294:C295"/>
+    <mergeCell ref="A134:A145"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="A94:A95"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C220:C221"/>
-    <mergeCell ref="A172:C172"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="A134:A145"/>
-    <mergeCell ref="C294:C295"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B310:B321"/>
     <mergeCell ref="C216:C217"/>
     <mergeCell ref="A262:A273"/>
-    <mergeCell ref="B18:B19"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="A122:A133"/>
     <mergeCell ref="C284:C285"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="C318:C319"/>
     <mergeCell ref="C280:C281"/>
     <mergeCell ref="B222:B233"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="A186:A197"/>
+    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C286:C287"/>
     <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C320:C321"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="C80:C81"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C246:C247"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C286:C287"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C202:C203"/>
-    <mergeCell ref="C320:C321"/>
     <mergeCell ref="C270:C271"/>
     <mergeCell ref="C192:C193"/>
     <mergeCell ref="A250:A261"/>
     <mergeCell ref="C144:C145"/>
     <mergeCell ref="A98:A109"/>
+    <mergeCell ref="C238:C239"/>
     <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C176:C177"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="C238:C239"/>
     <mergeCell ref="C70:C71"/>
     <mergeCell ref="C312:C313"/>
     <mergeCell ref="C194:C195"/>
     <mergeCell ref="A70:A81"/>
     <mergeCell ref="A82:A93"/>
     <mergeCell ref="C240:C241"/>
+    <mergeCell ref="C296:C297"/>
+    <mergeCell ref="C178:C179"/>
     <mergeCell ref="C122:C123"/>
+    <mergeCell ref="C78:C79"/>
     <mergeCell ref="B46:B57"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C296:C297"/>
     <mergeCell ref="C258:C259"/>
     <mergeCell ref="C314:C315"/>
     <mergeCell ref="A146:A157"/>
     <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="C106:C107"/>
     <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C224:C225"/>
     <mergeCell ref="C298:C299"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="B298:B309"/>
@@ -9907,8 +9908,8 @@
     <mergeCell ref="C170:C171"/>
     <mergeCell ref="C64:C65"/>
     <mergeCell ref="C204:C205"/>
+    <mergeCell ref="B274:B285"/>
     <mergeCell ref="A13:E13"/>
-    <mergeCell ref="B274:B285"/>
     <mergeCell ref="C154:C155"/>
     <mergeCell ref="B158:B169"/>
     <mergeCell ref="C212:C213"/>
@@ -9920,34 +9921,33 @@
     <mergeCell ref="C88:C89"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C302:C303"/>
     <mergeCell ref="C180:C181"/>
-    <mergeCell ref="C302:C303"/>
     <mergeCell ref="C118:C119"/>
     <mergeCell ref="A34:A45"/>
     <mergeCell ref="C198:C199"/>
     <mergeCell ref="C90:C91"/>
     <mergeCell ref="C130:C131"/>
     <mergeCell ref="C182:C183"/>
+    <mergeCell ref="B286:B297"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B286:B297"/>
+    <mergeCell ref="C110:C111"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="C232:C233"/>
     <mergeCell ref="C150:C151"/>
-    <mergeCell ref="C232:C233"/>
     <mergeCell ref="C72:C73"/>
     <mergeCell ref="C208:C209"/>
     <mergeCell ref="C158:C159"/>
     <mergeCell ref="C136:C137"/>
     <mergeCell ref="B262:B273"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C160:C161"/>
+    <mergeCell ref="C266:C267"/>
     <mergeCell ref="C260:C261"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="C186:C187"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C200:C201"/>
-    <mergeCell ref="C266:C267"/>
-    <mergeCell ref="B186:B197"/>
     <mergeCell ref="C92:C93"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13061,11 +13061,7 @@
           <t>11:40-13:10</t>
         </is>
       </c>
-      <c r="D240" s="45" t="inlineStr">
-        <is>
-          <t>Технологическая (проектно-технологическая) практика (Консультация)</t>
-        </is>
-      </c>
+      <c r="D240" s="45" t="inlineStr"/>
       <c r="E240" s="45" t="inlineStr">
         <is>
           <t>Исследование операций и методы оптимизации (СПЗ)</t>
@@ -13076,11 +13072,7 @@
       <c r="A241" s="30" t="n"/>
       <c r="B241" s="30" t="n"/>
       <c r="C241" s="42" t="n"/>
-      <c r="D241" s="46" t="inlineStr">
-        <is>
-          <t>Стряпунина Н.И.., ауд. 528</t>
-        </is>
-      </c>
+      <c r="D241" s="46" t="inlineStr"/>
       <c r="E241" s="46" t="inlineStr">
         <is>
           <t>зав.каф.Сурина Е.Е., ауд. 520</t>
@@ -13113,7 +13105,7 @@
       </c>
       <c r="E243" s="46" t="inlineStr"/>
     </row>
-    <row r="244" ht="12.75" customHeight="1">
+    <row r="244" ht="25.5" customHeight="1">
       <c r="A244" s="30" t="n"/>
       <c r="B244" s="30" t="n"/>
       <c r="C244" s="44" t="inlineStr">
@@ -13121,14 +13113,22 @@
           <t>15:25-16:55</t>
         </is>
       </c>
-      <c r="D244" s="37" t="inlineStr"/>
+      <c r="D244" s="45" t="inlineStr">
+        <is>
+          <t>Технологическая (проектно-технологическая) практика (Консультация)</t>
+        </is>
+      </c>
       <c r="E244" s="37" t="inlineStr"/>
     </row>
     <row r="245" ht="12.75" customHeight="1">
       <c r="A245" s="30" t="n"/>
       <c r="B245" s="30" t="n"/>
       <c r="C245" s="42" t="n"/>
-      <c r="D245" s="32" t="inlineStr"/>
+      <c r="D245" s="46" t="inlineStr">
+        <is>
+          <t>Преображенский М.В., ауд. 514</t>
+        </is>
+      </c>
       <c r="E245" s="32" t="inlineStr"/>
     </row>
     <row r="246" ht="12.75" customHeight="1">
@@ -13417,8 +13417,9 @@
     <mergeCell ref="C184:C185"/>
     <mergeCell ref="C250:C251"/>
     <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C234:C235"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C234:C235"/>
     <mergeCell ref="C134:C135"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C252:C253"/>
@@ -13431,15 +13432,15 @@
     <mergeCell ref="C132:C133"/>
     <mergeCell ref="B56:B67"/>
     <mergeCell ref="B184:B195"/>
+    <mergeCell ref="B236:B247"/>
     <mergeCell ref="C226:C227"/>
-    <mergeCell ref="B236:B247"/>
+    <mergeCell ref="C164:C165"/>
     <mergeCell ref="B32:B43"/>
-    <mergeCell ref="C164:C165"/>
     <mergeCell ref="B120:B131"/>
     <mergeCell ref="B80:B81"/>
     <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C228:C229"/>
     <mergeCell ref="B96:B107"/>
-    <mergeCell ref="C228:C229"/>
     <mergeCell ref="C222:C223"/>
     <mergeCell ref="C66:C67"/>
     <mergeCell ref="C262:C263"/>
@@ -13456,8 +13457,8 @@
     <mergeCell ref="A160:A171"/>
     <mergeCell ref="C98:C99"/>
     <mergeCell ref="C256:C257"/>
+    <mergeCell ref="A32:A43"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A32:A43"/>
     <mergeCell ref="C166:C167"/>
     <mergeCell ref="A224:A235"/>
     <mergeCell ref="B68:B79"/>
@@ -13466,31 +13467,31 @@
     <mergeCell ref="C218:C219"/>
     <mergeCell ref="C230:C231"/>
     <mergeCell ref="C112:C113"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A68:A79"/>
     <mergeCell ref="C168:C169"/>
     <mergeCell ref="A208:A209"/>
+    <mergeCell ref="A68:A79"/>
+    <mergeCell ref="C54:C55"/>
     <mergeCell ref="C100:C101"/>
     <mergeCell ref="C152:C153"/>
+    <mergeCell ref="A132:A143"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A132:A143"/>
     <mergeCell ref="C148:C149"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A260:A271"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C138:C139"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C120:C121"/>
     <mergeCell ref="A147:C147"/>
     <mergeCell ref="A148:A159"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B224:B235"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="B224:B235"/>
     <mergeCell ref="A84:A95"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C244:C245"/>
-    <mergeCell ref="C140:C141"/>
     <mergeCell ref="A211:C211"/>
     <mergeCell ref="A212:A223"/>
+    <mergeCell ref="C140:C141"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="A108:A119"/>
     <mergeCell ref="C268:C269"/>
@@ -13498,13 +13499,13 @@
     <mergeCell ref="C102:C103"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C126:C127"/>
     <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C126:C127"/>
     <mergeCell ref="A146:C146"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A20:A31"/>
+    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C116:C117"/>
     <mergeCell ref="B144:B145"/>
     <mergeCell ref="D144:E144"/>
@@ -13512,60 +13513,60 @@
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="A184:A195"/>
-    <mergeCell ref="A18:C18"/>
     <mergeCell ref="B208:B209"/>
     <mergeCell ref="D208:E208"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="B20:B31"/>
     <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="C84:C85"/>
     <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C22:C23"/>
     <mergeCell ref="A80:A81"/>
     <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A96:A107"/>
     <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A96:A107"/>
-    <mergeCell ref="C202:C203"/>
     <mergeCell ref="C270:C271"/>
     <mergeCell ref="C192:C193"/>
     <mergeCell ref="A144:A145"/>
     <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B248:B259"/>
     <mergeCell ref="C238:C239"/>
     <mergeCell ref="C176:C177"/>
-    <mergeCell ref="B248:B259"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="A172:A183"/>
     <mergeCell ref="C70:C71"/>
     <mergeCell ref="C194:C195"/>
-    <mergeCell ref="A56:A67"/>
+    <mergeCell ref="C240:C241"/>
     <mergeCell ref="C122:C123"/>
     <mergeCell ref="C178:C179"/>
-    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="A56:A67"/>
+    <mergeCell ref="A236:A247"/>
     <mergeCell ref="C78:C79"/>
-    <mergeCell ref="A236:A247"/>
     <mergeCell ref="C258:C259"/>
     <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="C106:C107"/>
     <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C224:C225"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C170:C171"/>
     <mergeCell ref="C64:C65"/>
     <mergeCell ref="C204:C205"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="C154:C155"/>
+    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C172:C173"/>
-    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C206:C207"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="C156:C157"/>
     <mergeCell ref="C196:C197"/>
     <mergeCell ref="B260:B271"/>
+    <mergeCell ref="B160:B171"/>
     <mergeCell ref="D80:E80"/>
-    <mergeCell ref="B160:B171"/>
     <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C124:C125"/>
     <mergeCell ref="C180:C181"/>
     <mergeCell ref="C118:C119"/>
@@ -13573,12 +13574,12 @@
     <mergeCell ref="C90:C91"/>
     <mergeCell ref="C130:C131"/>
     <mergeCell ref="C182:C183"/>
+    <mergeCell ref="C110:C111"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C110:C111"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="C150:C151"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="C232:C233"/>
     <mergeCell ref="B132:B143"/>
     <mergeCell ref="C72:C73"/>
     <mergeCell ref="C96:C97"/>
@@ -13587,14 +13588,13 @@
     <mergeCell ref="B148:B159"/>
     <mergeCell ref="C158:C159"/>
     <mergeCell ref="C136:C137"/>
+    <mergeCell ref="B84:B95"/>
     <mergeCell ref="B44:B55"/>
-    <mergeCell ref="B84:B95"/>
     <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C186:C187"/>
     <mergeCell ref="C108:C109"/>
-    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="C200:C201"/>
     <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C200:C201"/>
     <mergeCell ref="C266:C267"/>
     <mergeCell ref="C260:C261"/>
     <mergeCell ref="C92:C93"/>
@@ -17412,39 +17412,39 @@
   <mergeCells count="215">
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="B196:B207"/>
+    <mergeCell ref="C210:C211"/>
+    <mergeCell ref="C184:C185"/>
     <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C184:C185"/>
-    <mergeCell ref="C210:C211"/>
     <mergeCell ref="C250:C251"/>
     <mergeCell ref="C146:C147"/>
     <mergeCell ref="A156:A167"/>
+    <mergeCell ref="C234:C235"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="C274:C275"/>
     <mergeCell ref="C134:C135"/>
+    <mergeCell ref="C252:C253"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C252:C253"/>
-    <mergeCell ref="C274:C275"/>
     <mergeCell ref="B296:B307"/>
     <mergeCell ref="A220:A231"/>
     <mergeCell ref="A247:C247"/>
     <mergeCell ref="C114:C115"/>
     <mergeCell ref="C242:C243"/>
+    <mergeCell ref="C276:C277"/>
     <mergeCell ref="C236:C237"/>
-    <mergeCell ref="C276:C277"/>
     <mergeCell ref="C214:C215"/>
     <mergeCell ref="C132:C133"/>
     <mergeCell ref="B56:B67"/>
     <mergeCell ref="B184:B195"/>
     <mergeCell ref="C226:C227"/>
+    <mergeCell ref="B32:B43"/>
     <mergeCell ref="C164:C165"/>
-    <mergeCell ref="B32:B43"/>
     <mergeCell ref="C300:C301"/>
     <mergeCell ref="A171:C171"/>
     <mergeCell ref="C278:C279"/>
     <mergeCell ref="B120:B131"/>
     <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C228:C229"/>
     <mergeCell ref="B96:B107"/>
-    <mergeCell ref="C228:C229"/>
     <mergeCell ref="C222:C223"/>
     <mergeCell ref="C66:C67"/>
     <mergeCell ref="C262:C263"/>
@@ -17475,27 +17475,27 @@
     <mergeCell ref="C218:C219"/>
     <mergeCell ref="A168:A169"/>
     <mergeCell ref="C230:C231"/>
-    <mergeCell ref="C54:C55"/>
     <mergeCell ref="C112:C113"/>
+    <mergeCell ref="A308:A319"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="C168:C169"/>
     <mergeCell ref="A68:A79"/>
     <mergeCell ref="A95:C95"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="A308:A319"/>
+    <mergeCell ref="C54:C55"/>
     <mergeCell ref="C100:C101"/>
     <mergeCell ref="C152:C153"/>
+    <mergeCell ref="A132:A143"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A132:A143"/>
+    <mergeCell ref="C272:C273"/>
     <mergeCell ref="C148:C149"/>
-    <mergeCell ref="C272:C273"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A260:A271"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C282:C283"/>
     <mergeCell ref="C138:C139"/>
     <mergeCell ref="C316:C317"/>
+    <mergeCell ref="C120:C121"/>
     <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C120:C121"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A170:C170"/>
     <mergeCell ref="A284:A295"/>
@@ -17503,8 +17503,8 @@
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C244:C245"/>
     <mergeCell ref="B208:B219"/>
+    <mergeCell ref="C82:C83"/>
     <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C82:C83"/>
     <mergeCell ref="B168:B169"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="A108:A119"/>
@@ -17517,63 +17517,63 @@
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="A92:A93"/>
     <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C126:C127"/>
     <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C126:C127"/>
     <mergeCell ref="C310:C311"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A20:A31"/>
+    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C116:C117"/>
     <mergeCell ref="C294:C295"/>
     <mergeCell ref="C216:C217"/>
     <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="A184:A195"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A184:A195"/>
-    <mergeCell ref="C284:C285"/>
     <mergeCell ref="C318:C319"/>
     <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B284:B295"/>
+    <mergeCell ref="C280:C281"/>
     <mergeCell ref="B20:B31"/>
-    <mergeCell ref="C280:C281"/>
-    <mergeCell ref="B284:B295"/>
     <mergeCell ref="B244:B245"/>
     <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C84:C85"/>
     <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="C286:C287"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C286:C287"/>
     <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="C80:C81"/>
     <mergeCell ref="A96:A107"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C202:C203"/>
     <mergeCell ref="A232:A243"/>
     <mergeCell ref="C270:C271"/>
     <mergeCell ref="C192:C193"/>
     <mergeCell ref="B156:B167"/>
     <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B248:B259"/>
     <mergeCell ref="C238:C239"/>
     <mergeCell ref="C176:C177"/>
-    <mergeCell ref="B248:B259"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="A172:A183"/>
     <mergeCell ref="C70:C71"/>
     <mergeCell ref="C312:C313"/>
     <mergeCell ref="C194:C195"/>
     <mergeCell ref="B232:B243"/>
     <mergeCell ref="B272:B283"/>
+    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="C296:C297"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="C122:C123"/>
+    <mergeCell ref="C78:C79"/>
     <mergeCell ref="A56:A67"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="C240:C241"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C296:C297"/>
     <mergeCell ref="C258:C259"/>
     <mergeCell ref="C314:C315"/>
     <mergeCell ref="C48:C49"/>
     <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="C106:C107"/>
     <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C224:C225"/>
     <mergeCell ref="C298:C299"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C288:C289"/>
@@ -17581,8 +17581,8 @@
     <mergeCell ref="C204:C205"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="C154:C155"/>
+    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C172:C173"/>
-    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C206:C207"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="C156:C157"/>
@@ -17590,26 +17590,26 @@
     <mergeCell ref="C196:C197"/>
     <mergeCell ref="B260:B271"/>
     <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C124:C125"/>
+    <mergeCell ref="C302:C303"/>
     <mergeCell ref="C180:C181"/>
-    <mergeCell ref="C302:C303"/>
     <mergeCell ref="C118:C119"/>
     <mergeCell ref="B144:B155"/>
     <mergeCell ref="C198:C199"/>
     <mergeCell ref="C90:C91"/>
     <mergeCell ref="C130:C131"/>
     <mergeCell ref="C182:C183"/>
+    <mergeCell ref="C110:C111"/>
     <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="C150:C151"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="C232:C233"/>
     <mergeCell ref="B132:B143"/>
     <mergeCell ref="C72:C73"/>
+    <mergeCell ref="B220:B231"/>
     <mergeCell ref="C96:C97"/>
-    <mergeCell ref="B220:B231"/>
     <mergeCell ref="C208:C209"/>
     <mergeCell ref="A120:A131"/>
     <mergeCell ref="C158:C159"/>
@@ -17617,11 +17617,11 @@
     <mergeCell ref="A94:C94"/>
     <mergeCell ref="B44:B55"/>
     <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C186:C187"/>
     <mergeCell ref="C108:C109"/>
-    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C200:C201"/>
     <mergeCell ref="C266:C267"/>
     <mergeCell ref="C260:C261"/>
     <mergeCell ref="C92:C93"/>
@@ -21655,8 +21655,9 @@
     <mergeCell ref="C184:C185"/>
     <mergeCell ref="C250:C251"/>
     <mergeCell ref="C94:C95"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C234:C235"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C234:C235"/>
     <mergeCell ref="C134:C135"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C252:C253"/>
@@ -21669,15 +21670,15 @@
     <mergeCell ref="C132:C133"/>
     <mergeCell ref="B56:B67"/>
     <mergeCell ref="B184:B195"/>
+    <mergeCell ref="B236:B247"/>
     <mergeCell ref="C226:C227"/>
-    <mergeCell ref="B236:B247"/>
+    <mergeCell ref="C164:C165"/>
     <mergeCell ref="B32:B43"/>
-    <mergeCell ref="C164:C165"/>
     <mergeCell ref="B120:B131"/>
     <mergeCell ref="B80:B81"/>
     <mergeCell ref="C188:C189"/>
+    <mergeCell ref="C228:C229"/>
     <mergeCell ref="B96:B107"/>
-    <mergeCell ref="C228:C229"/>
     <mergeCell ref="C222:C223"/>
     <mergeCell ref="C66:C67"/>
     <mergeCell ref="C262:C263"/>
@@ -21708,31 +21709,31 @@
     <mergeCell ref="D208:H208"/>
     <mergeCell ref="C230:C231"/>
     <mergeCell ref="C112:C113"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A68:A79"/>
     <mergeCell ref="C168:C169"/>
     <mergeCell ref="A208:A209"/>
+    <mergeCell ref="A68:A79"/>
+    <mergeCell ref="C54:C55"/>
     <mergeCell ref="C100:C101"/>
     <mergeCell ref="C152:C153"/>
     <mergeCell ref="D146:F146"/>
+    <mergeCell ref="C56:C57"/>
     <mergeCell ref="A132:A143"/>
-    <mergeCell ref="C56:C57"/>
     <mergeCell ref="C148:C149"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A260:A271"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C138:C139"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C120:C121"/>
     <mergeCell ref="A147:C147"/>
     <mergeCell ref="A148:A159"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="C76:C77"/>
     <mergeCell ref="B224:B235"/>
     <mergeCell ref="A84:A95"/>
     <mergeCell ref="C60:C61"/>
     <mergeCell ref="C244:C245"/>
-    <mergeCell ref="C140:C141"/>
     <mergeCell ref="A211:C211"/>
     <mergeCell ref="A212:A223"/>
+    <mergeCell ref="C140:C141"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="A108:A119"/>
     <mergeCell ref="C268:C269"/>
@@ -21741,67 +21742,67 @@
     <mergeCell ref="C102:C103"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C74:C75"/>
+    <mergeCell ref="C126:C127"/>
     <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C126:C127"/>
     <mergeCell ref="A146:C146"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A20:A31"/>
+    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C220:C221"/>
     <mergeCell ref="C116:C117"/>
     <mergeCell ref="B144:B145"/>
     <mergeCell ref="C216:C217"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="A184:A195"/>
-    <mergeCell ref="A18:C18"/>
     <mergeCell ref="B208:B209"/>
     <mergeCell ref="D210:F210"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="B20:B31"/>
     <mergeCell ref="C50:C51"/>
+    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="C84:C85"/>
     <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="C22:C23"/>
     <mergeCell ref="A80:A81"/>
     <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C246:C247"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A96:A107"/>
     <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A96:A107"/>
-    <mergeCell ref="C202:C203"/>
     <mergeCell ref="C270:C271"/>
+    <mergeCell ref="C192:C193"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="C192:C193"/>
     <mergeCell ref="A144:A145"/>
+    <mergeCell ref="D84:H143"/>
     <mergeCell ref="C144:C145"/>
-    <mergeCell ref="D84:H143"/>
     <mergeCell ref="D20:G79"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="B248:B259"/>
     <mergeCell ref="C238:C239"/>
     <mergeCell ref="C176:C177"/>
-    <mergeCell ref="B248:B259"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="A172:A183"/>
     <mergeCell ref="C70:C71"/>
     <mergeCell ref="D82:F82"/>
     <mergeCell ref="C194:C195"/>
     <mergeCell ref="D16:H16"/>
+    <mergeCell ref="C240:C241"/>
     <mergeCell ref="A56:A67"/>
+    <mergeCell ref="C178:C179"/>
     <mergeCell ref="C122:C123"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="C240:C241"/>
+    <mergeCell ref="A236:A247"/>
     <mergeCell ref="C78:C79"/>
-    <mergeCell ref="A236:A247"/>
     <mergeCell ref="C258:C259"/>
     <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C224:C225"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="C106:C107"/>
-    <mergeCell ref="C224:C225"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C170:C171"/>
     <mergeCell ref="C64:C65"/>
     <mergeCell ref="C204:C205"/>
     <mergeCell ref="C154:C155"/>
+    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C172:C173"/>
-    <mergeCell ref="C212:C213"/>
     <mergeCell ref="C206:C207"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="C156:C157"/>
@@ -21809,8 +21810,8 @@
     <mergeCell ref="B260:B271"/>
     <mergeCell ref="B160:B171"/>
     <mergeCell ref="C88:C89"/>
+    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A44:A55"/>
     <mergeCell ref="C124:C125"/>
     <mergeCell ref="C180:C181"/>
     <mergeCell ref="C118:C119"/>
@@ -21818,12 +21819,12 @@
     <mergeCell ref="C90:C91"/>
     <mergeCell ref="C130:C131"/>
     <mergeCell ref="C182:C183"/>
+    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="C52:C53"/>
     <mergeCell ref="A12:H12"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="C232:C233"/>
+    <mergeCell ref="C150:C151"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="C232:C233"/>
     <mergeCell ref="B132:B143"/>
     <mergeCell ref="C72:C73"/>
     <mergeCell ref="C96:C97"/>
@@ -21832,15 +21833,14 @@
     <mergeCell ref="B148:B159"/>
     <mergeCell ref="C158:C159"/>
     <mergeCell ref="C136:C137"/>
-    <mergeCell ref="B44:B55"/>
     <mergeCell ref="B84:B95"/>
     <mergeCell ref="D212:H271"/>
+    <mergeCell ref="B44:B55"/>
     <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C186:C187"/>
     <mergeCell ref="C108:C109"/>
-    <mergeCell ref="C186:C187"/>
+    <mergeCell ref="C200:C201"/>
     <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C200:C201"/>
     <mergeCell ref="C266:C267"/>
     <mergeCell ref="C260:C261"/>
     <mergeCell ref="C92:C93"/>
@@ -25982,23 +25982,23 @@
     <mergeCell ref="C79:C80"/>
     <mergeCell ref="B143:B154"/>
     <mergeCell ref="C137:C138"/>
+    <mergeCell ref="C315:C316"/>
     <mergeCell ref="B183:B194"/>
-    <mergeCell ref="C315:C316"/>
+    <mergeCell ref="C29:C30"/>
     <mergeCell ref="B79:B90"/>
-    <mergeCell ref="C29:C30"/>
     <mergeCell ref="C225:C226"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="A143:A154"/>
     <mergeCell ref="C63:C64"/>
     <mergeCell ref="A243:A244"/>
     <mergeCell ref="C305:C306"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="A143:A154"/>
     <mergeCell ref="D171:D241"/>
     <mergeCell ref="A155:A166"/>
     <mergeCell ref="A67:A78"/>
     <mergeCell ref="C171:C172"/>
+    <mergeCell ref="C227:C228"/>
+    <mergeCell ref="C71:C72"/>
     <mergeCell ref="B95:B106"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C227:C228"/>
     <mergeCell ref="C123:C124"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="C211:C212"/>
@@ -26008,18 +26008,18 @@
     <mergeCell ref="C213:C214"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="A119:A130"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A93:C93"/>
     <mergeCell ref="C293:C294"/>
     <mergeCell ref="C149:C150"/>
+    <mergeCell ref="B259:B270"/>
     <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B259:B270"/>
     <mergeCell ref="A183:A194"/>
-    <mergeCell ref="B67:B78"/>
     <mergeCell ref="C199:C200"/>
     <mergeCell ref="A271:A282"/>
+    <mergeCell ref="B67:B78"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="A167:A168"/>
     <mergeCell ref="B231:B242"/>
@@ -26027,15 +26027,15 @@
     <mergeCell ref="A95:A106"/>
     <mergeCell ref="B91:B92"/>
     <mergeCell ref="C111:C112"/>
+    <mergeCell ref="B19:B30"/>
     <mergeCell ref="C151:C152"/>
-    <mergeCell ref="B19:B30"/>
     <mergeCell ref="C185:C186"/>
     <mergeCell ref="C191:C192"/>
     <mergeCell ref="C265:C266"/>
     <mergeCell ref="A131:A142"/>
     <mergeCell ref="A259:A270"/>
+    <mergeCell ref="A246:C246"/>
     <mergeCell ref="C175:C176"/>
-    <mergeCell ref="A246:C246"/>
     <mergeCell ref="B55:B66"/>
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="C85:C86"/>
@@ -26045,30 +26045,30 @@
     <mergeCell ref="A31:A42"/>
     <mergeCell ref="A43:A54"/>
     <mergeCell ref="A171:A182"/>
+    <mergeCell ref="C65:C66"/>
     <mergeCell ref="C109:C110"/>
-    <mergeCell ref="C65:C66"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="C201:C202"/>
     <mergeCell ref="C139:C140"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A107:A118"/>
-    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="C129:C130"/>
     <mergeCell ref="B31:B42"/>
     <mergeCell ref="C203:C204"/>
     <mergeCell ref="A170:C170"/>
+    <mergeCell ref="B307:B318"/>
+    <mergeCell ref="C297:C298"/>
+    <mergeCell ref="C51:C52"/>
     <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C297:C298"/>
-    <mergeCell ref="B307:B318"/>
     <mergeCell ref="C153:C154"/>
     <mergeCell ref="C131:C132"/>
     <mergeCell ref="C253:C254"/>
     <mergeCell ref="C267:C268"/>
     <mergeCell ref="B195:B206"/>
     <mergeCell ref="C299:C300"/>
+    <mergeCell ref="C181:C182"/>
     <mergeCell ref="A55:A66"/>
-    <mergeCell ref="C181:C182"/>
     <mergeCell ref="B219:B230"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C189:C190"/>
@@ -26078,27 +26078,27 @@
     <mergeCell ref="B283:B294"/>
     <mergeCell ref="C239:C240"/>
     <mergeCell ref="C83:C84"/>
+    <mergeCell ref="A247:A258"/>
+    <mergeCell ref="C49:C50"/>
     <mergeCell ref="C107:C108"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A247:A258"/>
     <mergeCell ref="C101:C102"/>
     <mergeCell ref="C229:C230"/>
+    <mergeCell ref="C221:C222"/>
     <mergeCell ref="B171:B182"/>
     <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C221:C222"/>
     <mergeCell ref="C73:C74"/>
     <mergeCell ref="B207:B218"/>
     <mergeCell ref="C113:C114"/>
     <mergeCell ref="C231:C232"/>
+    <mergeCell ref="C271:C272"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="C271:C272"/>
     <mergeCell ref="B271:B282"/>
     <mergeCell ref="C277:C278"/>
     <mergeCell ref="B167:B168"/>
     <mergeCell ref="C215:C216"/>
     <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C193:C194"/>
     <mergeCell ref="C115:C116"/>
-    <mergeCell ref="C193:C194"/>
     <mergeCell ref="C255:C256"/>
     <mergeCell ref="C295:C296"/>
     <mergeCell ref="C273:C274"/>
@@ -26123,9 +26123,9 @@
     <mergeCell ref="B119:B130"/>
     <mergeCell ref="C307:C308"/>
     <mergeCell ref="A12:D12"/>
+    <mergeCell ref="C283:C284"/>
+    <mergeCell ref="C217:C218"/>
     <mergeCell ref="C161:C162"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="C283:C284"/>
     <mergeCell ref="C195:C196"/>
     <mergeCell ref="C77:C78"/>
     <mergeCell ref="C235:C236"/>
@@ -26135,63 +26135,63 @@
     <mergeCell ref="C259:C260"/>
     <mergeCell ref="C141:C142"/>
     <mergeCell ref="C197:C198"/>
+    <mergeCell ref="A231:A242"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="C89:C90"/>
-    <mergeCell ref="A231:A242"/>
+    <mergeCell ref="C309:C310"/>
+    <mergeCell ref="C269:C270"/>
     <mergeCell ref="C187:C188"/>
-    <mergeCell ref="C269:C270"/>
-    <mergeCell ref="C309:C310"/>
     <mergeCell ref="C261:C262"/>
     <mergeCell ref="C143:C144"/>
+    <mergeCell ref="C205:C206"/>
     <mergeCell ref="A19:A30"/>
-    <mergeCell ref="C205:C206"/>
+    <mergeCell ref="B243:B244"/>
     <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B243:B244"/>
     <mergeCell ref="A295:A306"/>
     <mergeCell ref="C251:C252"/>
-    <mergeCell ref="C133:C134"/>
     <mergeCell ref="C75:C76"/>
     <mergeCell ref="C311:C312"/>
+    <mergeCell ref="C133:C134"/>
     <mergeCell ref="C127:C128"/>
     <mergeCell ref="C207:C208"/>
     <mergeCell ref="B131:B142"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="A79:A90"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="C117:C118"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="C301:C302"/>
+    <mergeCell ref="C55:C56"/>
     <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C301:C302"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="A207:A218"/>
     <mergeCell ref="D247:D317"/>
+    <mergeCell ref="B295:B306"/>
     <mergeCell ref="C163:C164"/>
-    <mergeCell ref="B295:B306"/>
     <mergeCell ref="C223:C224"/>
     <mergeCell ref="C67:C68"/>
     <mergeCell ref="C237:C238"/>
-    <mergeCell ref="C119:C120"/>
     <mergeCell ref="C61:C62"/>
     <mergeCell ref="B43:B54"/>
     <mergeCell ref="C303:C304"/>
+    <mergeCell ref="C119:C120"/>
     <mergeCell ref="C159:C160"/>
+    <mergeCell ref="C287:C288"/>
+    <mergeCell ref="A245:C245"/>
     <mergeCell ref="B155:B166"/>
     <mergeCell ref="C165:C166"/>
-    <mergeCell ref="A245:C245"/>
-    <mergeCell ref="C287:C288"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="B107:B118"/>
     <mergeCell ref="C125:C126"/>
-    <mergeCell ref="B107:B118"/>
-    <mergeCell ref="C81:C82"/>
     <mergeCell ref="C53:C54"/>
+    <mergeCell ref="A307:A318"/>
     <mergeCell ref="C289:C290"/>
-    <mergeCell ref="A307:A318"/>
+    <mergeCell ref="A94:C94"/>
     <mergeCell ref="C145:C146"/>
-    <mergeCell ref="A94:C94"/>
     <mergeCell ref="A283:A294"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C279:C280"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C279:C280"/>
     <mergeCell ref="C313:C314"/>
     <mergeCell ref="C147:C148"/>
     <mergeCell ref="A219:A230"/>
@@ -30779,54 +30779,54 @@
     <mergeCell ref="C79:C80"/>
     <mergeCell ref="B143:B154"/>
     <mergeCell ref="C137:C138"/>
+    <mergeCell ref="C315:C316"/>
     <mergeCell ref="A209:A220"/>
-    <mergeCell ref="C315:C316"/>
     <mergeCell ref="A169:A170"/>
+    <mergeCell ref="C29:C30"/>
     <mergeCell ref="B79:B90"/>
-    <mergeCell ref="C29:C30"/>
     <mergeCell ref="C225:C226"/>
+    <mergeCell ref="C63:C64"/>
     <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C305:C306"/>
     <mergeCell ref="A143:A154"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C305:C306"/>
     <mergeCell ref="A155:A168"/>
     <mergeCell ref="B185:B196"/>
     <mergeCell ref="A67:A78"/>
     <mergeCell ref="A247:C247"/>
+    <mergeCell ref="D173:F244"/>
+    <mergeCell ref="C227:C228"/>
+    <mergeCell ref="C71:C72"/>
     <mergeCell ref="B95:B106"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C227:C228"/>
-    <mergeCell ref="D173:F244"/>
     <mergeCell ref="C123:C124"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="C211:C212"/>
     <mergeCell ref="A91:A92"/>
     <mergeCell ref="C291:C292"/>
     <mergeCell ref="C173:C174"/>
+    <mergeCell ref="C213:C214"/>
     <mergeCell ref="A171:C171"/>
-    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="A197:A208"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A197:A208"/>
+    <mergeCell ref="F13:F14"/>
     <mergeCell ref="C105:C106"/>
-    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="A119:A130"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="A93:C93"/>
     <mergeCell ref="C293:C294"/>
     <mergeCell ref="C149:C150"/>
     <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C199:C200"/>
     <mergeCell ref="B67:B78"/>
-    <mergeCell ref="C199:C200"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="B169:B170"/>
     <mergeCell ref="C263:C264"/>
     <mergeCell ref="A95:A106"/>
+    <mergeCell ref="A273:A284"/>
     <mergeCell ref="B91:B92"/>
-    <mergeCell ref="A273:A284"/>
     <mergeCell ref="C111:C112"/>
+    <mergeCell ref="B19:B30"/>
     <mergeCell ref="C151:C152"/>
-    <mergeCell ref="B19:B30"/>
     <mergeCell ref="C185:C186"/>
     <mergeCell ref="C191:C192"/>
     <mergeCell ref="C265:C266"/>
@@ -30839,39 +30839,39 @@
     <mergeCell ref="D91:F91"/>
     <mergeCell ref="C281:C282"/>
     <mergeCell ref="A261:A272"/>
+    <mergeCell ref="A248:C248"/>
     <mergeCell ref="C177:C178"/>
-    <mergeCell ref="A248:C248"/>
     <mergeCell ref="A31:A42"/>
     <mergeCell ref="A43:A54"/>
+    <mergeCell ref="C65:C66"/>
     <mergeCell ref="C109:C110"/>
-    <mergeCell ref="C65:C66"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="C201:C202"/>
     <mergeCell ref="C139:C140"/>
+    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A107:A118"/>
-    <mergeCell ref="C31:C32"/>
     <mergeCell ref="A173:A184"/>
     <mergeCell ref="C129:C130"/>
+    <mergeCell ref="B233:B244"/>
     <mergeCell ref="B31:B42"/>
-    <mergeCell ref="B233:B244"/>
     <mergeCell ref="C203:C204"/>
+    <mergeCell ref="C297:C298"/>
+    <mergeCell ref="C51:C52"/>
     <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C297:C298"/>
     <mergeCell ref="C153:C154"/>
     <mergeCell ref="C131:C132"/>
     <mergeCell ref="B297:B308"/>
+    <mergeCell ref="D249:F320"/>
     <mergeCell ref="C253:C254"/>
-    <mergeCell ref="D249:F320"/>
     <mergeCell ref="C267:C268"/>
     <mergeCell ref="A221:A232"/>
     <mergeCell ref="C299:C300"/>
+    <mergeCell ref="C181:C182"/>
     <mergeCell ref="A55:A66"/>
-    <mergeCell ref="C181:C182"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C189:C190"/>
+    <mergeCell ref="C317:C318"/>
     <mergeCell ref="A11:F11"/>
-    <mergeCell ref="C317:C318"/>
     <mergeCell ref="C87:C88"/>
     <mergeCell ref="A245:A246"/>
     <mergeCell ref="C245:C246"/>
@@ -30879,27 +30879,27 @@
     <mergeCell ref="C239:C240"/>
     <mergeCell ref="C83:C84"/>
     <mergeCell ref="C319:C320"/>
+    <mergeCell ref="C49:C50"/>
     <mergeCell ref="C107:C108"/>
-    <mergeCell ref="C49:C50"/>
     <mergeCell ref="A185:A196"/>
-    <mergeCell ref="C101:C102"/>
     <mergeCell ref="A172:C172"/>
     <mergeCell ref="C229:C230"/>
+    <mergeCell ref="C101:C102"/>
     <mergeCell ref="C221:C222"/>
+    <mergeCell ref="B285:B296"/>
     <mergeCell ref="C103:C104"/>
-    <mergeCell ref="B285:B296"/>
     <mergeCell ref="C73:C74"/>
     <mergeCell ref="C113:C114"/>
+    <mergeCell ref="A249:A260"/>
     <mergeCell ref="C231:C232"/>
-    <mergeCell ref="A249:A260"/>
+    <mergeCell ref="C271:C272"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="C271:C272"/>
     <mergeCell ref="B173:B184"/>
     <mergeCell ref="C277:C278"/>
     <mergeCell ref="C215:C216"/>
     <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C193:C194"/>
     <mergeCell ref="C115:C116"/>
-    <mergeCell ref="C193:C194"/>
     <mergeCell ref="C255:C256"/>
     <mergeCell ref="C295:C296"/>
     <mergeCell ref="D245:F245"/>
@@ -30914,19 +30914,19 @@
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C169:C170"/>
     <mergeCell ref="C209:C210"/>
+    <mergeCell ref="B273:B284"/>
+    <mergeCell ref="C249:C250"/>
     <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C249:C250"/>
-    <mergeCell ref="B273:B284"/>
     <mergeCell ref="C243:C244"/>
+    <mergeCell ref="C39:C40"/>
     <mergeCell ref="B155:B168"/>
-    <mergeCell ref="C39:C40"/>
     <mergeCell ref="C233:C234"/>
     <mergeCell ref="C155:C156"/>
     <mergeCell ref="B119:B130"/>
     <mergeCell ref="C307:C308"/>
+    <mergeCell ref="C283:C284"/>
+    <mergeCell ref="C217:C218"/>
     <mergeCell ref="C161:C162"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="C283:C284"/>
     <mergeCell ref="C195:C196"/>
     <mergeCell ref="C77:C78"/>
     <mergeCell ref="C235:C236"/>
@@ -30938,33 +30938,33 @@
     <mergeCell ref="C141:C142"/>
     <mergeCell ref="C197:C198"/>
     <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B197:B208"/>
     <mergeCell ref="C89:C90"/>
-    <mergeCell ref="B197:B208"/>
+    <mergeCell ref="C309:C310"/>
+    <mergeCell ref="C269:C270"/>
     <mergeCell ref="C187:C188"/>
-    <mergeCell ref="C269:C270"/>
-    <mergeCell ref="C309:C310"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="C261:C262"/>
     <mergeCell ref="C143:C144"/>
-    <mergeCell ref="A19:A30"/>
     <mergeCell ref="C205:C206"/>
     <mergeCell ref="B309:B320"/>
+    <mergeCell ref="A19:A30"/>
     <mergeCell ref="B261:B272"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="C251:C252"/>
-    <mergeCell ref="C133:C134"/>
     <mergeCell ref="C75:C76"/>
     <mergeCell ref="C311:C312"/>
+    <mergeCell ref="C133:C134"/>
     <mergeCell ref="C127:C128"/>
     <mergeCell ref="C207:C208"/>
     <mergeCell ref="B131:B142"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="A79:A90"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="C117:C118"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="C301:C302"/>
+    <mergeCell ref="C55:C56"/>
     <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C301:C302"/>
     <mergeCell ref="B221:B232"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="D15:F15"/>
@@ -30972,29 +30972,29 @@
     <mergeCell ref="C223:C224"/>
     <mergeCell ref="C67:C68"/>
     <mergeCell ref="C237:C238"/>
-    <mergeCell ref="C119:C120"/>
     <mergeCell ref="C61:C62"/>
     <mergeCell ref="B43:B54"/>
+    <mergeCell ref="C303:C304"/>
     <mergeCell ref="D169:F169"/>
+    <mergeCell ref="C119:C120"/>
     <mergeCell ref="C159:C160"/>
-    <mergeCell ref="C303:C304"/>
     <mergeCell ref="B245:B246"/>
+    <mergeCell ref="C287:C288"/>
     <mergeCell ref="C165:C166"/>
-    <mergeCell ref="C287:C288"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="B107:B118"/>
     <mergeCell ref="C125:C126"/>
-    <mergeCell ref="B107:B118"/>
-    <mergeCell ref="C81:C82"/>
     <mergeCell ref="A233:A244"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="C289:C290"/>
+    <mergeCell ref="A94:C94"/>
     <mergeCell ref="C145:C146"/>
-    <mergeCell ref="A94:C94"/>
     <mergeCell ref="B249:B260"/>
     <mergeCell ref="A297:A308"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C279:C280"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C279:C280"/>
     <mergeCell ref="C313:C314"/>
     <mergeCell ref="C147:C148"/>
   </mergeCells>

</xml_diff>